<commit_message>
stopwords and equivalences for BIO dataset
</commit_message>
<xml_diff>
--- a/docs/Figuras.xlsx
+++ b/docs/Figuras.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/jarenas/github/edma-challenge/docs/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B0ECE56F-8AC3-CE46-B74C-4A46556CAEA6}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{65BE4706-B2F0-4646-B0C2-1F6F37EAC4FF}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="360" yWindow="60" windowWidth="28040" windowHeight="17440" activeTab="4" xr2:uid="{441E49F8-EBE9-FC4E-8232-A3ACE69645D0}"/>
+    <workbookView xWindow="360" yWindow="60" windowWidth="28040" windowHeight="17440" activeTab="3" xr2:uid="{441E49F8-EBE9-FC4E-8232-A3ACE69645D0}"/>
   </bookViews>
   <sheets>
     <sheet name="year Analysis" sheetId="1" r:id="rId1"/>
@@ -20,12 +20,6 @@
     <sheet name="Sheet2" sheetId="6" r:id="rId5"/>
     <sheet name="Sheet3" sheetId="7" r:id="rId6"/>
   </sheets>
-  <definedNames>
-    <definedName name="_xlchart.v1.0" hidden="1">Sheet2!$A$1:$A$40</definedName>
-    <definedName name="_xlchart.v1.1" hidden="1">Sheet2!$B$1:$B$40</definedName>
-    <definedName name="_xlchart.v1.2" hidden="1">Sheet2!$A$1:$A$40</definedName>
-    <definedName name="_xlchart.v1.3" hidden="1">Sheet2!$B$1:$B$40</definedName>
-  </definedNames>
   <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
@@ -44,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="78" uniqueCount="60">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="103" uniqueCount="85">
   <si>
     <t>Medicine</t>
   </si>
@@ -224,6 +218,81 @@
   </si>
   <si>
     <t>39 0.02003 enzyme inhibit reaction substrate acid bind study gst derivative biosynthesis synthase catalyze ligand residue result synthesize catalytic inhibition formation ring </t>
+  </si>
+  <si>
+    <t>0 0.03019 phosphorylation assay caspase Akt cell_cycle ERK PI3K cell_proliferation PTEN CDK Bax Bcl mouse MAPK cell_death JNK mTOR transfection actin Nrf </t>
+  </si>
+  <si>
+    <t>1 0.05747 membrane Ca peptide peptides intracellular calcium membranes assay PHEV fluorescence actin plasma_membrane vesicles localization transport extracellular degradation cytoplasm HSP rabbit </t>
+  </si>
+  <si>
+    <t>2 0.05857 genetic genes rs root iron roots tissues SNP tissue promoter transcript QTL vector genomes transcripts bp SNPs PCR gene_expression QTLs </t>
+  </si>
+  <si>
+    <t>3 0.05407 water nitrogen carbon uptake oxygen fertilization nitrate urea phosphorus graphene mineral degradation ammonia iron electron potassium ammonium curcumin Water transport </t>
+  </si>
+  <si>
+    <t>4 0.03134 infection IL mice HIV CD LPS HCV TLR HBV mouse ELISA influenza PCR TNF-α infections NS assay IFN-γ H5N immune_response </t>
+  </si>
+  <si>
+    <t>5 0.03458 tumor tumors HCC assay EGFR lung_cancer cancers cell_proliferation cisplatin PCR EMT VEGF NPC lung breast transfection CD STAT Smad gastric_cancer </t>
+  </si>
+  <si>
+    <t>6 0.01183 CRC MMP collagen FOXM ECM Cx Al Thellungiella PTH AFM GLUT CPB root_hair hair oxaliplatin HCT chitosan myeloma secretion earthworms </t>
+  </si>
+  <si>
+    <t>7 0.03652 glutathione MDA ascorbate peroxidase plants APX oxidative GST lipid hydrogen_peroxide catalase oxygen detoxification nitric_oxide malondialdehyde superoxide_dismutase water metabolism DHAR LOX </t>
+  </si>
+  <si>
+    <t>8 0.03478 rats glucose insulin cholesterol diabetes malaria obesity lipid liver serum mice blood hypertension rat animals ALT metformin AST creatinine leptin </t>
+  </si>
+  <si>
+    <t>9 0.02471 GFP Arabidopsis yeast CMV MPK localization PCR N._benthamiana MAPK plants YFP fluorescence tobacco assay TMV ubiquitin nucleus TRV transgenic MKK </t>
+  </si>
+  <si>
+    <t>10 0.0289 plants water NMR methanol ethanol quercetin methyl ethyl_acetate onion flavonoids alkaloids assay biosynthesis saponins chloroform antioxidant_activity Asteraceae ginseng cocoa hydroxy </t>
+  </si>
+  <si>
+    <t>11 0.03241 photosynthesis chlorophyll chloroplast PSII plants fluorescence chloroplasts electron lipid lipids transport plastid tocopherol Arabidopsis mitochondria photosystem membrane plastids NPQ oxygen </t>
+  </si>
+  <si>
+    <t>12 0.02617 insects cotton animals aphids AMF cattle plants bees birds bee pollination flies bats mammals humans coffee fish rodents oviposition behaviour </t>
+  </si>
+  <si>
+    <t>13 0.02022 biosynthesis Salmonella MYB sulfur flavonoid plants flavonoids glucoside glucosinolates Arabidopsis anthocyanins glucosinolate sulfate broccoli GLS cabbage ITC glucosides resveratrol metabolism </t>
+  </si>
+  <si>
+    <t>14 0.04612 PCR gene_expression methylation genetic assay chromosome MTA RNA-seq chromatin RNA-Seq nucleotides genes recombination chip insertion agarose histone CNV ChIP chromosomes </t>
+  </si>
+  <si>
+    <t>15 0.02507 plants maize soybean N._attenuata pea Ile nicotine M._sexta jasmonate insects biosynthesis Nicotiana_attenuata jasmonic_acid Nat Soybean PRR MYC Nova TPS CCA </t>
+  </si>
+  <si>
+    <t>16 0.03984 rice salt plants uptake water silicon transport arsenic metals Rice silica SOS Cd zinc plasma_membrane Silicon translocation Oryza_sativa alfalfa maize </t>
+  </si>
+  <si>
+    <t>17 0.02017 plants cucumber symbiosis chloroplast A._thaliana melatonin NBS land_plants LRR Arabidopsis HGT genetic plastid poplar eukaryotes P._patens PF rbcL M._truncatula L._japonicus </t>
+  </si>
+  <si>
+    <t>18 0.03556 stroke CT zebrafish depression uptake PET plague death asthma sleep anxiety iodine cardiac blood heart biopsy ischemic_stroke diabetes lymphoma heart_failure </t>
+  </si>
+  <si>
+    <t>19 0.05777 plants ABA Arabidopsis transgenic PCR water gene_expression NAC ethylene Plants tobacco biosynthesis salt GA abscisic_acid Arabidopsis_thaliana chlorophyll seed_germination CKX Transgenic </t>
+  </si>
+  <si>
+    <t>20 0.03538 plants tomato infection potato WRKY salicylic_acid Arabidopsis PR gene_expression SA PCR Tomato PVY ethylene nematodes nematode P._syringae Pst Solanum_lycopersicum tobacco </t>
+  </si>
+  <si>
+    <t>21 0.02855 PCR E._coli recombination sp Pseudomonas pig Escherichia_coli KX Proteobacteria phenanthrene Bacteria AB Actinobacteria MIC infection P._indica S._meliloti EU tetracycline M._ulcerans </t>
+  </si>
+  <si>
+    <t>22 0.0293 wheat barley chromosome cell_wall chromosomes D._citri maize apple rice durum_wheat Wheat cellulose glucan cell_walls polysaccharides banana lignin strawberry water oat </t>
+  </si>
+  <si>
+    <t>23 0.02396 mice autophagy mouse rats memory learning rat animals LC brain AMPK BMP morphine phosphorylation ATG rabbit SAH Notch Mice IL-1β </t>
+  </si>
+  <si>
+    <t>24 0.04224 metabolism glucose sucrose starch carbon PC biosynthesis glutamate nitrogen pyruvate fructose malate PCA amino_acids organic_acids aspartate transport citrate succinate fermentation </t>
   </si>
 </sst>
 </file>
@@ -3664,6 +3733,160 @@
           <c:extLst>
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
               <c16:uniqueId val="{00000000-32DF-4F41-958A-D20779833FA9}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:ser>
+          <c:idx val="1"/>
+          <c:order val="1"/>
+          <c:spPr>
+            <a:ln w="19050" cap="rnd">
+              <a:solidFill>
+                <a:schemeClr val="accent2"/>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="circle"/>
+            <c:size val="5"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent2"/>
+              </a:solidFill>
+              <a:ln w="9525">
+                <a:solidFill>
+                  <a:schemeClr val="accent2"/>
+                </a:solidFill>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+          </c:marker>
+          <c:xVal>
+            <c:numRef>
+              <c:f>Coherencia!$A$1:$A$17</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="17"/>
+                <c:pt idx="0">
+                  <c:v>25</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>30</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>40</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>50</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>60</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>75</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>100</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>125</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>150</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>175</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>200</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>250</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>300</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>350</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>400</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>450</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>500</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:xVal>
+          <c:yVal>
+            <c:numRef>
+              <c:f>Coherencia!$C$1:$C$17</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="17"/>
+                <c:pt idx="0">
+                  <c:v>0.58461308358171105</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>0.54476616999444805</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>0.57109607935126505</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>0.57025199868665899</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>0.56374850804311405</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>0.55460060642960196</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>0.56495927606107099</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>0.55849214517021695</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>0.574103098297578</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>0.57067254308780901</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>0.56427145052430505</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>0.56562818015179706</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>0.55561977432722098</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>0.56577433943022604</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>0.56985390554807402</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>0.55733466475777005</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>0.55565549094143596</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:yVal>
+          <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000001-B700-454E-9A9D-2A41F516907A}"/>
             </c:ext>
           </c:extLst>
         </c:ser>
@@ -10406,166 +10629,217 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8C786F57-9755-6245-805D-403EBFDCB926}">
-  <dimension ref="A1:B68"/>
+  <dimension ref="A1:C94"/>
   <sheetViews>
-    <sheetView topLeftCell="A28" workbookViewId="0">
-      <selection activeCell="A29" sqref="A29:A68"/>
+    <sheetView tabSelected="1" zoomScale="200" zoomScaleNormal="200" workbookViewId="0">
+      <selection activeCell="G63" sqref="G63"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A1">
         <v>25</v>
       </c>
       <c r="B1">
         <v>0.56129259542742604</v>
       </c>
-    </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="C1">
+        <v>0.58461308358171105</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A2">
         <v>30</v>
       </c>
       <c r="B2">
         <v>0.55238348046733898</v>
       </c>
-    </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="C2">
+        <v>0.54476616999444805</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A3">
         <v>40</v>
       </c>
       <c r="B3">
         <v>0.57676967317297001</v>
       </c>
-    </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="C3">
+        <v>0.57109607935126505</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A4">
         <v>50</v>
       </c>
       <c r="B4">
         <v>0.56738818077733599</v>
       </c>
-    </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="C4">
+        <v>0.57025199868665899</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A5">
         <v>60</v>
       </c>
       <c r="B5">
         <v>0.57326846010048904</v>
       </c>
-    </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="C5">
+        <v>0.56374850804311405</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A6">
         <v>75</v>
       </c>
       <c r="B6">
         <v>0.57359812477893202</v>
       </c>
-    </row>
-    <row r="7" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="C6">
+        <v>0.55460060642960196</v>
+      </c>
+    </row>
+    <row r="7" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A7">
         <v>100</v>
       </c>
       <c r="B7">
         <v>0.57005705729034195</v>
       </c>
-    </row>
-    <row r="8" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="C7">
+        <v>0.56495927606107099</v>
+      </c>
+    </row>
+    <row r="8" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A8">
         <v>125</v>
       </c>
       <c r="B8">
         <v>0.57644941962118501</v>
       </c>
-    </row>
-    <row r="9" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="C8">
+        <v>0.55849214517021695</v>
+      </c>
+    </row>
+    <row r="9" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A9">
         <v>150</v>
       </c>
       <c r="B9">
         <v>0.56494174649239803</v>
       </c>
-    </row>
-    <row r="10" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="C9">
+        <v>0.574103098297578</v>
+      </c>
+    </row>
+    <row r="10" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A10">
         <v>175</v>
       </c>
       <c r="B10">
         <v>0.559943813188859</v>
       </c>
-    </row>
-    <row r="11" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="C10">
+        <v>0.57067254308780901</v>
+      </c>
+    </row>
+    <row r="11" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A11">
         <v>200</v>
       </c>
       <c r="B11">
         <v>0.57151145370589695</v>
       </c>
-    </row>
-    <row r="12" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="C11">
+        <v>0.56427145052430505</v>
+      </c>
+    </row>
+    <row r="12" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A12">
         <v>250</v>
       </c>
       <c r="B12">
         <v>0.56651773632163505</v>
       </c>
-    </row>
-    <row r="13" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="C12">
+        <v>0.56562818015179706</v>
+      </c>
+    </row>
+    <row r="13" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A13">
         <v>300</v>
       </c>
       <c r="B13">
         <v>0.55720796931399397</v>
       </c>
-    </row>
-    <row r="14" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="C13">
+        <v>0.55561977432722098</v>
+      </c>
+    </row>
+    <row r="14" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A14">
         <v>350</v>
       </c>
       <c r="B14">
         <v>0.56603589400545395</v>
       </c>
-    </row>
-    <row r="15" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="C14">
+        <v>0.56577433943022604</v>
+      </c>
+    </row>
+    <row r="15" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A15">
         <v>400</v>
       </c>
       <c r="B15">
         <v>0.55960049683833402</v>
       </c>
-    </row>
-    <row r="16" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="C15">
+        <v>0.56985390554807402</v>
+      </c>
+    </row>
+    <row r="16" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A16">
         <v>450</v>
       </c>
       <c r="B16">
         <v>0.55784087948025296</v>
       </c>
-    </row>
-    <row r="17" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="C16">
+        <v>0.55733466475777005</v>
+      </c>
+    </row>
+    <row r="17" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A17">
         <v>500</v>
       </c>
       <c r="B17">
         <v>0.550615503049948</v>
       </c>
-    </row>
-    <row r="29" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="C17">
+        <v>0.55565549094143596</v>
+      </c>
+    </row>
+    <row r="29" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A29" s="3" t="s">
         <v>20</v>
       </c>
     </row>
-    <row r="30" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="30" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A30" s="3" t="s">
         <v>21</v>
       </c>
     </row>
-    <row r="31" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="31" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A31" s="3" t="s">
         <v>22</v>
       </c>
     </row>
-    <row r="32" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="32" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A32" s="3" t="s">
         <v>23</v>
       </c>
@@ -10748,6 +11022,131 @@
     <row r="68" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A68" s="3" t="s">
         <v>59</v>
+      </c>
+    </row>
+    <row r="70" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A70" s="3" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="71" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A71" s="3" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="72" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A72" s="3" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="73" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A73" s="3" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="74" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A74" s="3" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="75" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A75" s="3" t="s">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="76" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A76" s="3" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="77" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A77" s="3" t="s">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="78" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A78" s="3" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="79" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A79" s="3" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="80" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A80" s="3" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="81" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A81" s="3" t="s">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="82" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A82" s="3" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="83" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A83" s="3" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="84" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A84" s="3" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="85" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A85" s="3" t="s">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="86" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A86" s="3" t="s">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="87" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A87" s="3" t="s">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="88" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A88" s="3" t="s">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="89" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A89" s="3" t="s">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="90" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A90" s="3" t="s">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="91" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A91" s="3" t="s">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="92" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A92" s="3" t="s">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="93" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A93" s="3" t="s">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="94" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A94" s="3" t="s">
+        <v>84</v>
       </c>
     </row>
   </sheetData>
@@ -10760,7 +11159,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{614FB514-9354-9B48-8D11-61020067F1B8}">
   <dimension ref="A1:B40"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="K30" sqref="K30"/>
     </sheetView>
   </sheetViews>

</xml_diff>